<commit_message>
Atualização da planilha de requisitos
</commit_message>
<xml_diff>
--- a/Documentação/RequisitosPI.xlsx
+++ b/Documentação/RequisitosPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vit_o\projeto-pi-disel-2\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme Gotardo\Desktop\Projeto\projeto-pi-diesel-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B03C2E-9C4F-4E56-8307-201918F72736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5C0C10-8225-45C9-A137-694F7E8A42AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19E6C0FD-B2A9-43B6-AC9F-946FA7D45E18}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="205">
   <si>
     <t>Requisito</t>
   </si>
@@ -777,6 +777,33 @@
   </si>
   <si>
     <t>e oque vamos fazer a partir de hoje.</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>SP2</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>MÉDIA</t>
+  </si>
+  <si>
+    <t>Manual de Instalação do Projeto</t>
+  </si>
+  <si>
+    <t>Dashboards do ChartJS acessando o Banco de Dados</t>
+  </si>
+  <si>
+    <t>Procedimento com passo a passo da instalação do projeto</t>
+  </si>
+  <si>
+    <t>Integração dos dados do sensor no banco de dados</t>
   </si>
 </sst>
 </file>
@@ -921,7 +948,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -929,11 +956,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1010,22 +1117,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1035,49 +1126,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1090,6 +1141,99 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1154,6 +1298,823 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1080219104"/>
+        <c:axId val="1080218624"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1080219104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1080218624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1080218624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1080219104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161366</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4347882</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>107579</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8144B1A-2A95-6274-D75E-0CDC241C51A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1473,577 +2434,1285 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:Z121"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="63.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="26" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="55" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="32" t="s">
+      <c r="D3" s="59"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="H3" s="59"/>
+      <c r="I3" s="60"/>
+    </row>
+    <row r="4" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="32" t="s">
+      <c r="D4" s="59"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-    </row>
-    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+    </row>
+    <row r="5" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="32" t="s">
+      <c r="D5" s="59"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="H5" s="59"/>
+      <c r="I5" s="60"/>
+    </row>
+    <row r="6" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="32" t="s">
+      <c r="D6" s="59"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
+    </row>
+    <row r="7" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="32" t="s">
+      <c r="D7" s="59"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
+    </row>
+    <row r="8" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="32" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
+    </row>
+    <row r="9" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="32" t="s">
+      <c r="D9" s="59"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
+    </row>
+    <row r="10" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="32" t="s">
+      <c r="D10" s="59"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
+    </row>
+    <row r="11" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="32" t="s">
+      <c r="D11" s="59"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+    </row>
+    <row r="12" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="32" t="s">
+      <c r="D12" s="59"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+    </row>
+    <row r="13" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="32" t="s">
+      <c r="D13" s="59"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+    </row>
+    <row r="14" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="56" t="s">
         <v>167</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="57" t="s">
         <v>168</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="32" t="s">
+      <c r="D14" s="59"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
+    </row>
+    <row r="15" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="32" t="s">
+      <c r="D15" s="59"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="H15" s="59"/>
+      <c r="I15" s="60"/>
+    </row>
+    <row r="16" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="32" t="s">
+      <c r="D16" s="59"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="H16" s="59"/>
+      <c r="I16" s="60"/>
+    </row>
+    <row r="17" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="32" t="s">
+      <c r="D17" s="59"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="H17" s="59"/>
+      <c r="I17" s="60"/>
+    </row>
+    <row r="18" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="32" t="s">
+      <c r="D18" s="59"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="H18" s="59"/>
+      <c r="I18" s="60"/>
+    </row>
+    <row r="19" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="32" t="s">
+      <c r="D19" s="59"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-    </row>
-    <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="H19" s="59"/>
+      <c r="I19" s="60"/>
+    </row>
+    <row r="20" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="32" t="s">
+      <c r="D20" s="59"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="H20" s="59"/>
+      <c r="I20" s="60"/>
+    </row>
+    <row r="21" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="32" t="s">
+      <c r="D21" s="59"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="H21" s="59"/>
+      <c r="I21" s="60"/>
+    </row>
+    <row r="22" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="32" t="s">
+      <c r="D22" s="59"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="H22" s="59"/>
+      <c r="I22" s="60"/>
+    </row>
+    <row r="23" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="32" t="s">
+      <c r="D23" s="59"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="H23" s="59"/>
+      <c r="I23" s="60"/>
+    </row>
+    <row r="24" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="32" t="s">
+      <c r="D24" s="59"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="H24" s="59"/>
+      <c r="I24" s="60"/>
+    </row>
+    <row r="25" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="32" t="s">
+      <c r="D25" s="59"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="H25" s="59"/>
+      <c r="I25" s="60"/>
+    </row>
+    <row r="26" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="32" t="s">
+      <c r="D26" s="59"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-    </row>
-    <row r="27" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="H26" s="59"/>
+      <c r="I26" s="60"/>
+    </row>
+    <row r="27" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="2" t="s">
+      <c r="D27" s="59"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="61" t="s">
         <v>189</v>
       </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="H27" s="59"/>
+      <c r="I27" s="60"/>
+    </row>
+    <row r="28" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="D28" s="62"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="61" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="H28" s="62"/>
+      <c r="I28" s="63"/>
+    </row>
+    <row r="29" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="56" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="62"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="66" t="s">
+        <v>189</v>
+      </c>
+      <c r="H29" s="62"/>
+      <c r="I29" s="63"/>
+    </row>
+    <row r="30" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="56" t="s">
+        <v>202</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="C30" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="62"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="66" t="s">
+        <v>189</v>
+      </c>
+      <c r="H30" s="62"/>
+      <c r="I30" s="63"/>
+    </row>
+    <row r="31" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="64" t="s">
         <v>185</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B31" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C31" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="D31" s="67"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="66" t="s">
         <v>189</v>
       </c>
+      <c r="H31" s="67"/>
+      <c r="I31" s="68"/>
+    </row>
+    <row r="32" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="48"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="E32" s="31"/>
+      <c r="G32" s="49"/>
+    </row>
+    <row r="33" spans="1:7" s="8" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="48"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="71" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="72">
+        <v>86</v>
+      </c>
+      <c r="E33" s="31"/>
+      <c r="G33" s="49"/>
+    </row>
+    <row r="34" spans="1:7" s="8" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="69" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="73">
+        <f>SUMIF(G3:G31,G15,E3:E31)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="31"/>
+      <c r="G34" s="49"/>
+    </row>
+    <row r="35" spans="1:7" s="8" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="69" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="73">
+        <f>SUMIF(G3:G31,G5,E3:E31)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="G35" s="49"/>
+    </row>
+    <row r="36" spans="1:7" s="8" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="48"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="69" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="73">
+        <f>SUMIF(G3:G31,G27,E3:E31)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="31"/>
+      <c r="G36" s="49"/>
+    </row>
+    <row r="37" spans="1:7" s="8" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="48"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="70" t="s">
+        <v>200</v>
+      </c>
+      <c r="D37" s="74">
+        <f>AVERAGE(D34,D35,D36)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="31"/>
+      <c r="G37" s="49"/>
+    </row>
+    <row r="38" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="E38" s="31"/>
+      <c r="G38" s="49"/>
+    </row>
+    <row r="39" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="E39" s="31"/>
+      <c r="G39" s="49"/>
+    </row>
+    <row r="40" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="48"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="E40" s="31"/>
+      <c r="G40" s="49"/>
+    </row>
+    <row r="41" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="48"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="E41" s="31"/>
+      <c r="G41" s="49"/>
+    </row>
+    <row r="42" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="48"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="E42" s="31"/>
+      <c r="G42" s="49"/>
+    </row>
+    <row r="43" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="48"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="E43" s="31"/>
+      <c r="G43" s="49"/>
+    </row>
+    <row r="44" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="48"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="E44" s="31"/>
+      <c r="G44" s="49"/>
+    </row>
+    <row r="45" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="48"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="E45" s="31"/>
+      <c r="G45" s="49"/>
+    </row>
+    <row r="46" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="48"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="E46" s="31"/>
+      <c r="G46" s="49"/>
+    </row>
+    <row r="47" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="48"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="E47" s="31"/>
+      <c r="G47" s="49"/>
+    </row>
+    <row r="48" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="48"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="E48" s="31"/>
+      <c r="G48" s="49"/>
+    </row>
+    <row r="49" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="48"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="E49" s="31"/>
+      <c r="G49" s="49"/>
+    </row>
+    <row r="50" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="48"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="E50" s="31"/>
+      <c r="G50" s="49"/>
+    </row>
+    <row r="51" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="48"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="E51" s="31"/>
+      <c r="G51" s="49"/>
+    </row>
+    <row r="52" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="48"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="E52" s="31"/>
+      <c r="G52" s="49"/>
+    </row>
+    <row r="53" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="48"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="E53" s="31"/>
+      <c r="G53" s="49"/>
+    </row>
+    <row r="54" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="48"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="E54" s="31"/>
+      <c r="G54" s="49"/>
+    </row>
+    <row r="55" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="48"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="49"/>
+      <c r="E55" s="31"/>
+      <c r="G55" s="49"/>
+    </row>
+    <row r="56" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="48"/>
+      <c r="B56" s="49"/>
+      <c r="C56" s="49"/>
+      <c r="E56" s="31"/>
+      <c r="G56" s="49"/>
+    </row>
+    <row r="57" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="48"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
+      <c r="E57" s="31"/>
+      <c r="G57" s="49"/>
+    </row>
+    <row r="58" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="48"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
+      <c r="E58" s="31"/>
+      <c r="G58" s="49"/>
+    </row>
+    <row r="59" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="48"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="49"/>
+      <c r="E59" s="31"/>
+      <c r="G59" s="49"/>
+    </row>
+    <row r="60" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="48"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="49"/>
+      <c r="E60" s="31"/>
+      <c r="G60" s="49"/>
+    </row>
+    <row r="61" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="48"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="E61" s="31"/>
+      <c r="G61" s="49"/>
+    </row>
+    <row r="62" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="48"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="49"/>
+      <c r="E62" s="31"/>
+      <c r="G62" s="49"/>
+    </row>
+    <row r="63" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="E63" s="31"/>
+      <c r="G63" s="49"/>
+    </row>
+    <row r="64" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="48"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="49"/>
+      <c r="E64" s="31"/>
+      <c r="G64" s="49"/>
+    </row>
+    <row r="65" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="48"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="E65" s="31"/>
+      <c r="G65" s="49"/>
+    </row>
+    <row r="66" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="48"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="E66" s="31"/>
+      <c r="G66" s="49"/>
+    </row>
+    <row r="67" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="48"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="49"/>
+      <c r="E67" s="31"/>
+      <c r="G67" s="49"/>
+    </row>
+    <row r="68" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="48"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
+      <c r="E68" s="31"/>
+      <c r="G68" s="49"/>
+    </row>
+    <row r="69" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="48"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="49"/>
+      <c r="E69" s="31"/>
+      <c r="G69" s="49"/>
+    </row>
+    <row r="70" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="48"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="49"/>
+      <c r="E70" s="31"/>
+      <c r="G70" s="49"/>
+    </row>
+    <row r="71" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="48"/>
+      <c r="B71" s="49"/>
+      <c r="C71" s="49"/>
+      <c r="E71" s="31"/>
+      <c r="G71" s="49"/>
+    </row>
+    <row r="72" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="48"/>
+      <c r="B72" s="49"/>
+      <c r="C72" s="49"/>
+      <c r="E72" s="31"/>
+      <c r="G72" s="49"/>
+    </row>
+    <row r="73" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="48"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="49"/>
+      <c r="E73" s="31"/>
+      <c r="G73" s="49"/>
+    </row>
+    <row r="74" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="48"/>
+      <c r="B74" s="49"/>
+      <c r="C74" s="49"/>
+      <c r="E74" s="31"/>
+      <c r="G74" s="49"/>
+    </row>
+    <row r="75" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="48"/>
+      <c r="B75" s="49"/>
+      <c r="C75" s="49"/>
+      <c r="E75" s="31"/>
+      <c r="G75" s="49"/>
+    </row>
+    <row r="76" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="48"/>
+      <c r="B76" s="49"/>
+      <c r="C76" s="49"/>
+      <c r="E76" s="31"/>
+      <c r="G76" s="49"/>
+    </row>
+    <row r="77" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="48"/>
+      <c r="B77" s="49"/>
+      <c r="C77" s="49"/>
+      <c r="E77" s="31"/>
+      <c r="G77" s="49"/>
+    </row>
+    <row r="78" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="48"/>
+      <c r="B78" s="49"/>
+      <c r="C78" s="49"/>
+      <c r="E78" s="31"/>
+      <c r="G78" s="49"/>
+    </row>
+    <row r="79" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="48"/>
+      <c r="B79" s="49"/>
+      <c r="C79" s="49"/>
+      <c r="E79" s="31"/>
+      <c r="G79" s="49"/>
+    </row>
+    <row r="80" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="48"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="49"/>
+      <c r="E80" s="31"/>
+      <c r="G80" s="49"/>
+    </row>
+    <row r="81" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="48"/>
+      <c r="B81" s="49"/>
+      <c r="C81" s="49"/>
+      <c r="E81" s="31"/>
+      <c r="G81" s="49"/>
+    </row>
+    <row r="82" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="48"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="E82" s="31"/>
+      <c r="G82" s="49"/>
+    </row>
+    <row r="83" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="48"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="49"/>
+      <c r="E83" s="31"/>
+      <c r="G83" s="49"/>
+    </row>
+    <row r="84" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="48"/>
+      <c r="B84" s="49"/>
+      <c r="C84" s="49"/>
+      <c r="E84" s="31"/>
+      <c r="G84" s="49"/>
+    </row>
+    <row r="85" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="48"/>
+      <c r="B85" s="49"/>
+      <c r="C85" s="49"/>
+      <c r="E85" s="31"/>
+      <c r="G85" s="49"/>
+    </row>
+    <row r="86" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="48"/>
+      <c r="B86" s="49"/>
+      <c r="C86" s="49"/>
+      <c r="E86" s="31"/>
+      <c r="G86" s="49"/>
+    </row>
+    <row r="87" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="48"/>
+      <c r="B87" s="49"/>
+      <c r="C87" s="49"/>
+      <c r="E87" s="31"/>
+      <c r="G87" s="49"/>
+    </row>
+    <row r="88" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="48"/>
+      <c r="B88" s="49"/>
+      <c r="C88" s="49"/>
+      <c r="E88" s="31"/>
+      <c r="G88" s="49"/>
+    </row>
+    <row r="89" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="48"/>
+      <c r="B89" s="49"/>
+      <c r="C89" s="49"/>
+      <c r="E89" s="31"/>
+      <c r="G89" s="49"/>
+    </row>
+    <row r="90" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="48"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="49"/>
+      <c r="E90" s="31"/>
+      <c r="G90" s="49"/>
+    </row>
+    <row r="91" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="48"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="49"/>
+      <c r="E91" s="31"/>
+      <c r="G91" s="49"/>
+    </row>
+    <row r="92" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="48"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="49"/>
+      <c r="E92" s="31"/>
+      <c r="G92" s="49"/>
+    </row>
+    <row r="93" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="48"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="49"/>
+      <c r="E93" s="31"/>
+      <c r="G93" s="49"/>
+    </row>
+    <row r="94" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="48"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="49"/>
+      <c r="E94" s="31"/>
+      <c r="G94" s="49"/>
+    </row>
+    <row r="95" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="48"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="49"/>
+      <c r="E95" s="31"/>
+      <c r="G95" s="49"/>
+    </row>
+    <row r="96" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="48"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="49"/>
+      <c r="E96" s="31"/>
+      <c r="G96" s="49"/>
+    </row>
+    <row r="97" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="48"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="49"/>
+      <c r="E97" s="31"/>
+      <c r="G97" s="49"/>
+    </row>
+    <row r="98" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="48"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="49"/>
+      <c r="E98" s="31"/>
+      <c r="G98" s="49"/>
+    </row>
+    <row r="99" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="48"/>
+      <c r="B99" s="49"/>
+      <c r="C99" s="49"/>
+      <c r="E99" s="31"/>
+      <c r="G99" s="49"/>
+    </row>
+    <row r="100" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="48"/>
+      <c r="B100" s="49"/>
+      <c r="C100" s="49"/>
+      <c r="E100" s="31"/>
+      <c r="G100" s="49"/>
+    </row>
+    <row r="101" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="48"/>
+      <c r="B101" s="49"/>
+      <c r="C101" s="49"/>
+      <c r="E101" s="31"/>
+      <c r="G101" s="49"/>
+    </row>
+    <row r="102" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="48"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="49"/>
+      <c r="E102" s="31"/>
+      <c r="G102" s="49"/>
+    </row>
+    <row r="103" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="48"/>
+      <c r="B103" s="49"/>
+      <c r="C103" s="49"/>
+      <c r="E103" s="31"/>
+      <c r="G103" s="49"/>
+    </row>
+    <row r="104" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="48"/>
+      <c r="B104" s="49"/>
+      <c r="C104" s="49"/>
+      <c r="E104" s="31"/>
+      <c r="G104" s="49"/>
+    </row>
+    <row r="105" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="48"/>
+      <c r="B105" s="49"/>
+      <c r="C105" s="49"/>
+      <c r="E105" s="31"/>
+      <c r="G105" s="49"/>
+    </row>
+    <row r="106" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="48"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="49"/>
+      <c r="E106" s="31"/>
+      <c r="G106" s="49"/>
+    </row>
+    <row r="107" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="48"/>
+      <c r="B107" s="49"/>
+      <c r="C107" s="49"/>
+      <c r="E107" s="31"/>
+      <c r="G107" s="49"/>
+    </row>
+    <row r="108" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="48"/>
+      <c r="B108" s="49"/>
+      <c r="C108" s="49"/>
+      <c r="E108" s="31"/>
+      <c r="G108" s="49"/>
+    </row>
+    <row r="109" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="48"/>
+      <c r="B109" s="49"/>
+      <c r="C109" s="49"/>
+      <c r="E109" s="31"/>
+      <c r="G109" s="49"/>
+    </row>
+    <row r="110" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="48"/>
+      <c r="B110" s="49"/>
+      <c r="C110" s="49"/>
+      <c r="E110" s="31"/>
+      <c r="G110" s="49"/>
+    </row>
+    <row r="111" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="48"/>
+      <c r="B111" s="49"/>
+      <c r="C111" s="49"/>
+      <c r="E111" s="31"/>
+      <c r="G111" s="49"/>
+    </row>
+    <row r="112" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="48"/>
+      <c r="B112" s="49"/>
+      <c r="C112" s="49"/>
+      <c r="E112" s="31"/>
+      <c r="G112" s="49"/>
+    </row>
+    <row r="113" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="48"/>
+      <c r="B113" s="49"/>
+      <c r="C113" s="49"/>
+      <c r="E113" s="31"/>
+      <c r="G113" s="49"/>
+    </row>
+    <row r="114" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="48"/>
+      <c r="B114" s="49"/>
+      <c r="C114" s="49"/>
+      <c r="E114" s="31"/>
+      <c r="G114" s="49"/>
+    </row>
+    <row r="115" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="48"/>
+      <c r="B115" s="49"/>
+      <c r="C115" s="49"/>
+      <c r="E115" s="31"/>
+      <c r="G115" s="49"/>
+    </row>
+    <row r="116" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="48"/>
+      <c r="B116" s="49"/>
+      <c r="C116" s="49"/>
+      <c r="E116" s="31"/>
+      <c r="G116" s="49"/>
+    </row>
+    <row r="117" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="48"/>
+      <c r="B117" s="49"/>
+      <c r="C117" s="49"/>
+      <c r="E117" s="31"/>
+      <c r="G117" s="49"/>
+    </row>
+    <row r="118" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="48"/>
+      <c r="B118" s="49"/>
+      <c r="C118" s="49"/>
+      <c r="E118" s="31"/>
+      <c r="G118" s="49"/>
+    </row>
+    <row r="119" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="48"/>
+      <c r="B119" s="49"/>
+      <c r="C119" s="49"/>
+      <c r="E119" s="31"/>
+      <c r="G119" s="49"/>
+    </row>
+    <row r="120" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="48"/>
+      <c r="B120" s="49"/>
+      <c r="C120" s="49"/>
+      <c r="E120" s="31"/>
+      <c r="G120" s="49"/>
+    </row>
+    <row r="121" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="48"/>
+      <c r="B121" s="49"/>
+      <c r="C121" s="49"/>
+      <c r="E121" s="31"/>
+      <c r="G121" s="49"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:I2" xr:uid="{8E066C66-EDC5-4576-81E7-7D26CF0E3E63}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D2:I2 C2:C1048576">
+  <conditionalFormatting sqref="D2:I2 C40:C1048576 C2:C37">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"ESSENCIAL"</formula>
     </cfRule>
@@ -2061,6 +3730,7 @@
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2068,16 +3738,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94C5F1C-D311-4CF6-87DF-957E92D912B8}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -2096,11 +3766,11 @@
       <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="42" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -2119,9 +3789,9 @@
       <c r="F2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="40"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -2144,7 +3814,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
@@ -2167,7 +3837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -2190,7 +3860,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>34</v>
       </c>
@@ -2213,7 +3883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -2234,7 +3904,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
@@ -2255,7 +3925,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -2276,7 +3946,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>3</v>
       </c>
@@ -2297,7 +3967,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>52</v>
       </c>
@@ -2318,7 +3988,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>56</v>
       </c>
@@ -2339,7 +4009,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>59</v>
       </c>
@@ -2360,7 +4030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>63</v>
       </c>
@@ -2381,7 +4051,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
@@ -2402,7 +4072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -2423,7 +4093,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>74</v>
       </c>
@@ -2472,120 +4142,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841281C-2601-4B0A-8C45-7CFA6831C0EC}">
   <dimension ref="A1:AH59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" customWidth="1"/>
-    <col min="13" max="13" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="7" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="3.33203125" customWidth="1"/>
+    <col min="13" max="13" width="30.6640625" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" customWidth="1"/>
-    <col min="19" max="19" width="26.28515625" customWidth="1"/>
-    <col min="25" max="25" width="5.5703125" customWidth="1"/>
-    <col min="26" max="26" width="3.7109375" customWidth="1"/>
-    <col min="34" max="34" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" customWidth="1"/>
+    <col min="19" max="19" width="26.33203125" customWidth="1"/>
+    <col min="25" max="25" width="5.5546875" customWidth="1"/>
+    <col min="26" max="26" width="3.6640625" customWidth="1"/>
+    <col min="34" max="34" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="12"/>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="M1" s="41" t="s">
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="M1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="46">
         <v>45554</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="13"/>
       <c r="G2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="46">
         <v>45555</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
       <c r="M2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="42">
+      <c r="N2" s="46">
         <v>45557</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
       <c r="F3" s="14"/>
       <c r="G3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
       <c r="M3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>81</v>
       </c>
@@ -2608,7 +4278,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>84</v>
       </c>
@@ -2631,7 +4301,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>83</v>
       </c>
@@ -2652,7 +4322,7 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>85</v>
       </c>
@@ -2671,7 +4341,7 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>86</v>
       </c>
@@ -2690,7 +4360,7 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>193</v>
       </c>
@@ -2713,59 +4383,59 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A10" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="52" t="s">
+      <c r="D10" s="43"/>
+      <c r="E10" s="10" t="s">
         <v>89</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44" t="s">
+      <c r="H10" s="43"/>
+      <c r="I10" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="J10" s="44"/>
+      <c r="J10" s="43"/>
       <c r="K10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="M10" s="44" t="s">
+      <c r="M10" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44" t="s">
+      <c r="N10" s="43"/>
+      <c r="O10" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="P10" s="44"/>
+      <c r="P10" s="43"/>
       <c r="Q10" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A11" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54">
+      <c r="D11" s="44"/>
+      <c r="E11" s="11">
         <v>45560</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
       <c r="K11" s="11"/>
       <c r="M11" s="22" t="s">
         <v>90</v>
@@ -2781,23 +4451,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A12" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="54">
+      <c r="D12" s="44"/>
+      <c r="E12" s="11">
         <v>45560</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
       <c r="K12" s="11"/>
       <c r="M12" s="19" t="s">
         <v>91</v>
@@ -2813,23 +4483,23 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A13" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="54">
+      <c r="D13" s="44"/>
+      <c r="E13" s="11">
         <v>45560</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
       <c r="K13" s="11"/>
       <c r="M13" s="19" t="s">
         <v>92</v>
@@ -2845,16 +4515,16 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="53" t="s">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A14" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54">
+      <c r="D14" s="44"/>
+      <c r="E14" s="11">
         <v>45560</v>
       </c>
       <c r="G14" s="8"/>
@@ -2876,7 +4546,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
@@ -2894,7 +4564,6 @@
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
-      <c r="R15" s="55"/>
       <c r="AA15" s="17"/>
       <c r="AB15" s="17"/>
       <c r="AC15" s="17"/>
@@ -2904,147 +4573,147 @@
       <c r="AG15" s="17"/>
       <c r="AH15" s="17"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="G16" s="41" t="s">
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="G16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="M16" s="41" t="s">
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="M16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="AA16" s="41" t="s">
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="AA16" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="AB16" s="41"/>
-      <c r="AC16" s="41"/>
-      <c r="AD16" s="41"/>
-      <c r="AE16" s="41"/>
-      <c r="AF16" s="41"/>
-      <c r="AG16" s="41"/>
-      <c r="AH16" s="41"/>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AB16" s="45"/>
+      <c r="AC16" s="45"/>
+      <c r="AD16" s="45"/>
+      <c r="AE16" s="45"/>
+      <c r="AF16" s="45"/>
+      <c r="AG16" s="45"/>
+      <c r="AH16" s="45"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="46">
         <v>45558</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
       <c r="G17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="42">
+      <c r="H17" s="46">
         <v>45559</v>
       </c>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="M17" s="38" t="s">
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="M17" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="N17" s="42">
+      <c r="N17" s="46">
         <v>45560</v>
       </c>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
       <c r="AA17" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AB17" s="42">
+      <c r="AB17" s="46">
         <v>45564</v>
       </c>
-      <c r="AC17" s="42"/>
-      <c r="AD17" s="42"/>
-      <c r="AE17" s="42"/>
+      <c r="AC17" s="46"/>
+      <c r="AD17" s="46"/>
+      <c r="AE17" s="46"/>
       <c r="AF17" s="8"/>
       <c r="AG17" s="8"/>
       <c r="AH17" s="8"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
       <c r="G18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="43" t="s">
+      <c r="H18" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="M18" s="38" t="s">
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="M18" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="43" t="s">
+      <c r="N18" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
       <c r="AA18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AB18" s="38" t="s">
+      <c r="AB18" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AC18" s="38"/>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="38"/>
+      <c r="AC18" s="32"/>
+      <c r="AD18" s="32"/>
+      <c r="AE18" s="32"/>
       <c r="AF18" s="8"/>
       <c r="AG18" s="8"/>
       <c r="AH18" s="8"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="AA19" s="46"/>
-      <c r="AB19" s="46"/>
-      <c r="AC19" s="46"/>
-      <c r="AD19" s="46"/>
-      <c r="AE19" s="46"/>
-      <c r="AF19" s="46"/>
-      <c r="AG19" s="46"/>
-      <c r="AH19" s="46"/>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>81</v>
       </c>
@@ -3072,12 +4741,12 @@
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
       <c r="AD20" s="9"/>
-      <c r="AE20" s="48"/>
-      <c r="AF20" s="48"/>
-      <c r="AG20" s="48"/>
-      <c r="AH20" s="48"/>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>112</v>
       </c>
@@ -3110,7 +4779,7 @@
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>111</v>
       </c>
@@ -3141,7 +4810,7 @@
       <c r="AG22" s="8"/>
       <c r="AH22" s="8"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>113</v>
       </c>
@@ -3170,7 +4839,7 @@
       <c r="AG23" s="8"/>
       <c r="AH23" s="8"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -3195,7 +4864,7 @@
       <c r="AG24" s="8"/>
       <c r="AH24" s="8"/>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>193</v>
       </c>
@@ -3226,11 +4895,11 @@
       <c r="AG25" s="9"/>
       <c r="AH25" s="9"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A26" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="44"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="18" t="s">
         <v>88</v>
       </c>
@@ -3240,10 +4909,10 @@
       <c r="E26" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="44" t="s">
+      <c r="G26" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="44"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="18" t="s">
         <v>88</v>
       </c>
@@ -3253,10 +4922,10 @@
       <c r="K26" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="M26" s="44" t="s">
+      <c r="M26" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="N26" s="44"/>
+      <c r="N26" s="43"/>
       <c r="O26" s="18" t="s">
         <v>88</v>
       </c>
@@ -3275,25 +4944,24 @@
       <c r="AG26" s="10"/>
       <c r="AH26" s="10"/>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A27" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="58"/>
-      <c r="C27" s="59" t="s">
+      <c r="B27" s="36"/>
+      <c r="C27" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="59" t="s">
+      <c r="D27" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="E27" s="60">
+      <c r="E27" s="38">
         <v>45560</v>
       </c>
-      <c r="F27" s="55"/>
-      <c r="G27" s="62" t="s">
+      <c r="G27" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="H27" s="62"/>
+      <c r="H27" s="40"/>
       <c r="I27" s="27" t="s">
         <v>115</v>
       </c>
@@ -3303,7 +4971,6 @@
       <c r="K27" s="28">
         <v>45560</v>
       </c>
-      <c r="L27" s="55"/>
       <c r="M27" s="25" t="s">
         <v>128</v>
       </c>
@@ -3326,25 +4993,24 @@
       <c r="AG27" s="25"/>
       <c r="AH27" s="25"/>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28" s="58" t="s">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A28" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="59" t="s">
+      <c r="B28" s="36"/>
+      <c r="C28" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="60">
+      <c r="E28" s="38">
         <v>45560</v>
       </c>
-      <c r="F28" s="55"/>
-      <c r="G28" s="62" t="s">
+      <c r="G28" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="H28" s="62"/>
+      <c r="H28" s="40"/>
       <c r="I28" s="27" t="s">
         <v>122</v>
       </c>
@@ -3354,7 +5020,6 @@
       <c r="K28" s="28">
         <v>45560</v>
       </c>
-      <c r="L28" s="55"/>
       <c r="M28" s="25" t="s">
         <v>129</v>
       </c>
@@ -3377,11 +5042,11 @@
       <c r="AG28" s="25"/>
       <c r="AH28" s="25"/>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A29" s="63" t="s">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A29" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="63"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="25" t="s">
         <v>117</v>
       </c>
@@ -3391,11 +5056,10 @@
       <c r="E29" s="26">
         <v>45560</v>
       </c>
-      <c r="F29" s="55"/>
-      <c r="G29" s="62" t="s">
+      <c r="G29" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="H29" s="62"/>
+      <c r="H29" s="40"/>
       <c r="I29" s="27" t="s">
         <v>117</v>
       </c>
@@ -3405,7 +5069,6 @@
       <c r="K29" s="28">
         <v>45560</v>
       </c>
-      <c r="L29" s="55"/>
       <c r="M29" s="25" t="s">
         <v>130</v>
       </c>
@@ -3428,11 +5091,11 @@
       <c r="AG29" s="25"/>
       <c r="AH29" s="25"/>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A30" s="63" t="s">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A30" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="63"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="25" t="s">
         <v>121</v>
       </c>
@@ -3442,11 +5105,10 @@
       <c r="E30" s="26">
         <v>45565</v>
       </c>
-      <c r="F30" s="55"/>
-      <c r="G30" s="62" t="s">
+      <c r="G30" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="62"/>
+      <c r="H30" s="40"/>
       <c r="I30" s="27" t="s">
         <v>121</v>
       </c>
@@ -3456,7 +5118,6 @@
       <c r="K30" s="28">
         <v>45565</v>
       </c>
-      <c r="L30" s="55"/>
       <c r="M30" s="25" t="s">
         <v>131</v>
       </c>
@@ -3479,19 +5140,17 @@
       <c r="AG30" s="25"/>
       <c r="AH30" s="25"/>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="55"/>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
       <c r="M31" s="27" t="s">
         <v>101</v>
       </c>
@@ -3514,7 +5173,7 @@
       <c r="AG31" s="25"/>
       <c r="AH31" s="25"/>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -3541,79 +5200,75 @@
       <c r="AG32" s="17"/>
       <c r="AH32" s="17"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="41" t="s">
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="33"/>
+      <c r="G33" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="36">
+      <c r="B34" s="30">
         <v>45561</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="55"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
       <c r="G34" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H34" s="42">
+      <c r="H34" s="46">
         <v>45563</v>
       </c>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="55"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
       <c r="G35" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H35" s="43" t="s">
+      <c r="H35" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>81</v>
       </c>
@@ -3621,7 +5276,6 @@
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="55"/>
       <c r="G37" s="9" t="s">
         <v>81</v>
       </c>
@@ -3630,7 +5284,7 @@
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>194</v>
       </c>
@@ -3638,7 +5292,6 @@
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
-      <c r="F38" s="55"/>
       <c r="G38" s="8" t="s">
         <v>190</v>
       </c>
@@ -3647,7 +5300,7 @@
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>195</v>
       </c>
@@ -3655,7 +5308,6 @@
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="55"/>
       <c r="G39" s="8" t="s">
         <v>191</v>
       </c>
@@ -3664,33 +5316,31 @@
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="55"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="55"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>193</v>
       </c>
@@ -3698,14 +5348,12 @@
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="44"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="18" t="s">
         <v>88</v>
       </c>
@@ -3715,70 +5363,91 @@
       <c r="E43" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F43" s="55"/>
-      <c r="G43" s="56"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="25"/>
       <c r="B44" s="25"/>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
       <c r="E44" s="26"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="57"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G44" s="35"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="25"/>
       <c r="B45" s="25"/>
       <c r="C45" s="25"/>
       <c r="D45" s="25"/>
       <c r="E45" s="26"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="57"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G45" s="35"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="25"/>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
       <c r="D46" s="25"/>
       <c r="E46" s="26"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="57"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G46" s="35"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="25"/>
       <c r="B47" s="25"/>
       <c r="C47" s="25"/>
       <c r="D47" s="25"/>
       <c r="E47" s="26"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="57"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G47" s="35"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="25"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
       <c r="D48" s="25"/>
       <c r="E48" s="26"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="57"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G48" s="35"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R59" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="AB17:AE17"/>
+    <mergeCell ref="AA16:AH16"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="G26:H26"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
@@ -3795,35 +5464,6 @@
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="AB17:AE17"/>
-    <mergeCell ref="AA16:AH16"/>
-    <mergeCell ref="A33:D33"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>